<commit_message>
core-jdbc & common-daoの変更取り込み (#33)
* core-jdbc & common-daoの変更取り込み
</commit_message>
<xml_diff>
--- a/src/test/java/com/nablarch/example/app/web/action/ProjectBulkActionRequestTest.xlsx
+++ b/src/test/java/com/nablarch/example/app/web/action/ProjectBulkActionRequestTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="23565" windowHeight="5190" tabRatio="766"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="23565" windowHeight="5190" tabRatio="766" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="setUpDb" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="203">
   <si>
     <t>LIST_MAP=user</t>
     <phoneticPr fontId="2"/>
@@ -632,10 +632,6 @@
   </si>
   <si>
     <t>searchForm.sortKey</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>name</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -1754,7 +1750,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="10" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleSheetLayoutView="10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1789,7 +1785,7 @@
     </row>
     <row r="3" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1797,64 +1793,64 @@
     </row>
     <row r="4" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="39" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="C4" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="D4" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="E4" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="F4" s="39" t="s">
         <v>182</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="G4" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="H4" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="I4" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="I4" s="39" t="s">
+      <c r="J4" s="39" t="s">
         <v>186</v>
-      </c>
-      <c r="J4" s="39" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" s="35" t="s">
         <v>188</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="C5" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="D5" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="E5" s="50" t="s">
         <v>191</v>
       </c>
-      <c r="E5" s="50" t="s">
+      <c r="F5" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="G5" s="42" t="s">
         <v>193</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="H5" s="42" t="s">
         <v>194</v>
-      </c>
-      <c r="H5" s="42" t="s">
-        <v>195</v>
       </c>
       <c r="I5" s="51"/>
       <c r="J5" s="42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.35">
@@ -1862,7 +1858,7 @@
     </row>
     <row r="7" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1870,25 +1866,25 @@
     </row>
     <row r="8" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="39" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="C8" s="39" t="s">
         <v>198</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>199</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="B9" s="31" t="s">
         <v>200</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="C9" s="31" t="s">
         <v>201</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>202</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -2352,7 +2348,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>2</v>
@@ -2369,7 +2365,7 @@
       <c r="G4" s="36"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:256" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.5">
@@ -3156,7 +3152,7 @@
     </row>
     <row r="10" spans="1:256" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A10" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>22</v>
@@ -3961,7 +3957,7 @@
     </row>
     <row r="18" spans="1:256" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
@@ -4233,7 +4229,9 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV88"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleSheetLayoutView="10" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleSheetLayoutView="10" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4556,7 +4554,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>2</v>
@@ -5104,7 +5102,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -5368,7 +5366,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -5626,7 +5624,7 @@
     </row>
     <row r="11" spans="1:256" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A11" s="49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B11" s="22"/>
       <c r="C11" s="17"/>
@@ -7171,9 +7169,7 @@
       <c r="A35" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="31" t="s">
-        <v>124</v>
-      </c>
+      <c r="B35" s="31"/>
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
       <c r="G35" s="19"/>
@@ -8602,7 +8598,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>2</v>
@@ -9150,7 +9146,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -9414,7 +9410,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -9672,7 +9668,7 @@
     </row>
     <row r="11" spans="1:256" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A11" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B11" s="22"/>
       <c r="C11" s="17"/>
@@ -10387,7 +10383,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:255" s="6" customFormat="1" ht="22.5" x14ac:dyDescent="0.35">
@@ -10656,7 +10652,7 @@
     </row>
     <row r="24" spans="1:255" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:255" x14ac:dyDescent="0.35">
@@ -11230,7 +11226,7 @@
         <v>86</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
@@ -16454,7 +16450,7 @@
     </row>
     <row r="65" spans="1:256" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E65" s="19"/>
       <c r="F65" s="19"/>
@@ -16711,7 +16707,7 @@
     </row>
     <row r="66" spans="1:256" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="67" spans="1:256" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -20598,7 +20594,7 @@
     </row>
     <row r="83" spans="1:256" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E83" s="19"/>
       <c r="F83" s="19"/>
@@ -20855,7 +20851,7 @@
     </row>
     <row r="84" spans="1:256" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="85" spans="1:256" x14ac:dyDescent="0.35">
@@ -22543,7 +22539,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>2</v>
@@ -22556,7 +22552,7 @@
         <v>59</v>
       </c>
       <c r="G4" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
@@ -23091,7 +23087,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -23355,7 +23351,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -23613,7 +23609,7 @@
     </row>
     <row r="11" spans="1:256" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A11" s="49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B11" s="22"/>
       <c r="C11" s="17"/>
@@ -24758,7 +24754,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>2</v>
@@ -24775,7 +24771,7 @@
       <c r="G4" s="36"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:256" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.5">
@@ -26517,22 +26513,22 @@
         <v>8</v>
       </c>
       <c r="B19" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="C19" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="F19" s="30" t="s">
+      <c r="G19" s="30" t="s">
         <v>143</v>
-      </c>
-      <c r="G19" s="30" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:256" ht="15" x14ac:dyDescent="0.35">
@@ -26540,22 +26536,22 @@
         <v>1</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C20" s="43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D20" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="E20" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="E20" s="42" t="s">
-        <v>139</v>
-      </c>
       <c r="F20" s="43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G20" s="43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:256" s="6" customFormat="1" ht="22.5" x14ac:dyDescent="0.35">
@@ -26819,7 +26815,7 @@
     </row>
     <row r="23" spans="1:256" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
@@ -27076,7 +27072,7 @@
     </row>
     <row r="24" spans="1:256" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:256" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -27344,7 +27340,7 @@
         <v>44</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
@@ -30963,7 +30959,7 @@
     </row>
     <row r="41" spans="1:256" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:256" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -31231,7 +31227,7 @@
         <v>44</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E43" s="19"/>
       <c r="F43" s="19"/>
@@ -35185,7 +35181,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>2</v>
@@ -35200,11 +35196,11 @@
         <v>59</v>
       </c>
       <c r="G4" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:256" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.5">
@@ -36946,22 +36942,22 @@
         <v>8</v>
       </c>
       <c r="B19" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="C19" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="F19" s="30" t="s">
+      <c r="G19" s="30" t="s">
         <v>143</v>
-      </c>
-      <c r="G19" s="30" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:255" ht="15" x14ac:dyDescent="0.35">
@@ -36970,19 +36966,19 @@
       </c>
       <c r="B20" s="46"/>
       <c r="C20" s="43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D20" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="E20" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="E20" s="42" t="s">
-        <v>139</v>
-      </c>
       <c r="F20" s="43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G20" s="43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:255" s="6" customFormat="1" ht="22.5" x14ac:dyDescent="0.35">
@@ -37580,7 +37576,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>2</v>
@@ -37597,7 +37593,7 @@
       <c r="G4" s="36"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:256" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.5">
@@ -38384,7 +38380,7 @@
     </row>
     <row r="10" spans="1:256" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A10" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>22</v>
@@ -39611,7 +39607,7 @@
     </row>
     <row r="23" spans="1:256" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
@@ -39868,7 +39864,7 @@
     </row>
     <row r="24" spans="1:256" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:256" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -40136,7 +40132,7 @@
         <v>44</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
@@ -43755,7 +43751,7 @@
     </row>
     <row r="41" spans="1:256" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:256" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -44541,7 +44537,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E45" s="19"/>
       <c r="F45" s="19"/>
@@ -46349,7 +46345,7 @@
         <v>86</v>
       </c>
       <c r="B52" s="31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E52" s="19"/>
       <c r="F52" s="19"/>
@@ -47458,7 +47454,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>2</v>
@@ -47470,12 +47466,12 @@
         <v>1</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:256" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.5">
@@ -48262,7 +48258,7 @@
     </row>
     <row r="10" spans="1:256" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A10" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>22</v>
@@ -48846,7 +48842,7 @@
     </row>
     <row r="14" spans="1:256" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="44" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B14" s="40" t="s">
         <v>39</v>
@@ -48896,7 +48892,7 @@
     </row>
     <row r="15" spans="1:256" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B15" s="40" t="s">
         <v>101</v>
@@ -49489,7 +49485,7 @@
     </row>
     <row r="23" spans="1:256" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
@@ -49810,10 +49806,10 @@
     </row>
     <row r="26" spans="1:256" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="44" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C26" s="40" t="s">
         <v>40</v>
@@ -49860,10 +49856,10 @@
     </row>
     <row r="27" spans="1:256" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C27" s="40" t="s">
         <v>40</v>
@@ -50244,13 +50240,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>1</v>
@@ -50259,11 +50255,11 @@
         <v>59</v>
       </c>
       <c r="G4" s="36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:256" s="21" customFormat="1" ht="22.5" x14ac:dyDescent="0.5">
@@ -51050,7 +51046,7 @@
     </row>
     <row r="10" spans="1:256" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.4">
       <c r="A10" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>22</v>

</xml_diff>